<commit_message>
getting potential distribution partner details from IDIS
</commit_message>
<xml_diff>
--- a/email_extractor/output/Extraction_27to30Jan26_PreMQL.xlsx
+++ b/email_extractor/output/Extraction_27to30Jan26_PreMQL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agrawalapurw\Documents\LM_Automation\email_extractor\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FC4E2E-5F69-42F3-BBF1-103258C6078B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB6A3B8-716E-4754-90C9-C56E065B207F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7963,17 +7963,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AY1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BA156" sqref="BA156"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="50" customWidth="1"/>
-    <col min="2" max="2" width="30" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="22" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="50" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="50" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
     <col min="7" max="7" width="44" customWidth="1"/>
@@ -26938,7 +26938,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:BF169" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="A28:AZ28 BB28:BF28 A2:BF5 A29:BF31 A8:BF11 A6:AX6 AZ6:BF6 A13:BF27 A12:AX12 AZ12:BF12 A39:BF55 A38:AX38 AZ38:BF38 A104:BF111 A102:AX102 AZ102:BF102 A116:BF121 A114:AX115 AZ114:BF115 A137:BF141 A136:AX136 AZ136:BF136 A143:BF153 A142:AX142 AZ142:BF142 A7:AY7 BA7:BF7 A33:BF37 A32:AY32 BA32:BF32 A57:BF68 A56:AY56 BA56:BF56 A70:BF95 A69:AY69 BA69:BF69 A97:BF101 A96:AY96 BA96:BF96 A103:AY103 BA103:BF103 A112:AY113 BA112:BF113 A123:BF135 A122:AY122 BA122:BF122 A157:BF164 A154:AY156 BA154:BF156 A166:BF169 A165:AY165 BA165:BF165">
+  <conditionalFormatting sqref="A2:BF5 A6:AX6 AZ6:BF6 A7:AY7 BA7:BF7 A8:BF11 A12:AX12 AZ12:BF12 A13:BF27 A28:AZ28 BB28:BF28 A29:BF31 A32:AY32 BA32:BF32 A33:BF37 A38:AX38 AZ38:BF38 A39:BF55 A56:AY56 BA56:BF56 A57:BF68 A69:AY69 BA69:BF69 A70:BF95 A96:AY96 BA96:BF96 A97:BF101 A102:AX102 AZ102:BF102 A103:AY103 BA103:BF103 A104:BF111 A112:AY113 BA112:BF113 A114:AX115 AZ114:BF115 A116:BF121 A122:AY122 BA122:BF122 A123:BF135 A136:AX136 AZ136:BF136 A137:BF141 A142:AX142 AZ142:BF142 A143:BF153 A154:AY156 BA154:BF156 A157:BF164 A165:AY165 BA165:BF165 A166:BF169">
     <cfRule type="expression" dxfId="18" priority="674">
       <formula>$BC2="EBV/Avnet"</formula>
     </cfRule>
@@ -26958,7 +26958,7 @@
       <formula>$BC2="Rejected Marketing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BB28:BF28 A28:AZ28 A2:BF5 A29:BF31 A8:BF11 A6:AX6 AZ6:BF6 A13:BF27 A12:AX12 AZ12:BF12 A39:BF55 A38:AX38 AZ38:BF38 A104:BF111 A102:AX102 AZ102:BF102 A116:BF121 A114:AX115 AZ114:BF115 A137:BF141 A136:AX136 AZ136:BF136 A143:BF153 A142:AX142 AZ142:BF142 A7:AY7 BA7:BF7 A33:BF37 A32:AY32 BA32:BF32 A57:BF68 A56:AY56 BA56:BF56 A70:BF95 A69:AY69 BA69:BF69 A97:BF101 A96:AY96 BA96:BF96 A103:AY103 BA103:BF103 A112:AY113 BA112:BF113 A123:BF135 A122:AY122 BA122:BF122 A157:BF164 A154:AY156 BA154:BF156 A166:BF169 A165:AY165 BA165:BF165">
+  <conditionalFormatting sqref="A2:BF5 AZ6:BF6 BA7:BF7 A8:BF11 AZ12:BF12 A13:BF27 BB28:BF28 A29:BF31 BA32:BF32 A33:BF37 AZ38:BF38 A39:BF55 BA56:BF56 A57:BF68 BA69:BF69 A70:BF95 BA96:BF96 A97:BF101 AZ102:BF102 BA103:BF103 A104:BF111 BA112:BF113 AZ114:BF115 A116:BF121 BA122:BF122 A123:BF135 AZ136:BF136 A137:BF141 AZ142:BF142 A143:BF153 BA154:BF156 A157:BF164 BA165:BF165 A166:BF169 A28:AZ28 A7:AY7 A32:AY32 A56:AY56 A69:AY69 A96:AY96 A103:AY103 A112:AY113 A122:AY122 A154:AY156 A165:AY165 A6:AX6 A12:AX12 A38:AX38 A102:AX102 A114:AX115 A136:AX136 A142:AX142">
     <cfRule type="expression" dxfId="12" priority="673">
       <formula>$BC2="Arrow"</formula>
     </cfRule>

</xml_diff>